<commit_message>
Add: Momentary Pushbutton Switch.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\MediaController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0278ED3-0969-4C9C-B052-83144AAB365C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7761D537-B4D6-40A0-A162-214218C03BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="115">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -363,6 +363,15 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/vishay-dale/RCG060310K0JNEA/541-1804-1-ND/4172563</t>
+  </si>
+  <si>
+    <t>Reset Switches</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/c-k/D6R90-F1-LFS/401-1978-ND/1466335</t>
+  </si>
+  <si>
+    <t>401-1978-ND</t>
   </si>
 </sst>
 </file>
@@ -575,10 +584,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -590,16 +605,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -957,7 +966,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,57 +978,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="L1" s="23" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="L1" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="24" t="s">
+      <c r="M2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1028,16 +1037,16 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>104</v>
@@ -1045,57 +1054,57 @@
       <c r="L3" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="29" t="s">
+      <c r="M3" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
       <c r="S3" s="19"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
       <c r="K4" t="s">
         <v>103</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="29" t="s">
+      <c r="M4" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="22"/>
       <c r="S4" s="19"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24" t="s">
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1104,54 +1113,54 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="22"/>
       <c r="S7" s="19"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24" t="s">
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1160,72 +1169,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="L10" s="23" t="s">
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="L10" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="24" t="s">
+      <c r="M11" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24" t="s">
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1234,27 +1243,27 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="26" t="s">
+      <c r="M12" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1278,64 +1287,64 @@
       <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="L15" s="23" t="s">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="L15" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
-      <c r="S15" s="23"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="24" t="s">
+      <c r="M16" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="24" t="s">
+      <c r="N16" s="26"/>
+      <c r="O16" s="26"/>
+      <c r="P16" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="26"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1344,62 +1353,88 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
       <c r="L17" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="M17" s="29" t="s">
+      <c r="M17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
       <c r="S17" s="19"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L18" s="19"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
       <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="L19" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
       <c r="H20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M20" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1407,49 +1442,61 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="26" t="s">
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
       <c r="I21" t="s">
         <v>41</v>
       </c>
+      <c r="L21" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="M21" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="N21" s="22"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="22"/>
+      <c r="S21" s="19"/>
     </row>
     <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24" t="s">
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1458,76 +1505,76 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24" t="s">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="24" t="s">
+      <c r="B31" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24" t="s">
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1539,16 +1586,16 @@
       <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="26" t="s">
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -1557,128 +1604,154 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="25"/>
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24" t="s">
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24" t="s">
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="22"/>
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
       <c r="H41" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
+  <mergeCells count="85">
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="A7:H7"/>
@@ -1695,49 +1768,28 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="A15:H15"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{29E80626-A7A5-45E8-8609-3380F35C4604}"/>
@@ -1762,9 +1814,10 @@
     <hyperlink ref="M17" r:id="rId20" xr:uid="{D29D4C77-7913-4955-AB7D-07B2251F19FD}"/>
     <hyperlink ref="B14" r:id="rId21" xr:uid="{8FA66079-3753-47E9-B090-2503163763E2}"/>
     <hyperlink ref="M12" r:id="rId22" xr:uid="{0A036A2D-396A-4563-AA5D-8BAE50337625}"/>
+    <hyperlink ref="M21" r:id="rId23" xr:uid="{487E3C3E-3BEA-4A39-8CC2-A2E909E780A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId23"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add: 1uF 0603 Capacitor.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7761D537-B4D6-40A0-A162-214218C03BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673AED6E-97F9-45D6-93D6-6448749DBC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -372,6 +372,27 @@
   </si>
   <si>
     <t>401-1978-ND</t>
+  </si>
+  <si>
+    <t>1uF Caps</t>
+  </si>
+  <si>
+    <t>C0603C105K8PACTU</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/kemet/C0603C105K8PACTU/399-3118-1-ND/551623</t>
+  </si>
+  <si>
+    <t>0.1uF Caps</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/kemet/C0603C104Z3VACTU/399-1100-1-ND/411375</t>
+  </si>
+  <si>
+    <t>C0603C104Z3VACTU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -966,7 +987,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="P7" sqref="P7:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,7 +1080,9 @@
       </c>
       <c r="N3" s="22"/>
       <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
+      <c r="P3" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="Q3" s="22"/>
       <c r="R3" s="22"/>
       <c r="S3" s="19"/>
@@ -1086,7 +1109,9 @@
       </c>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
+      <c r="P4" s="22" t="s">
+        <v>121</v>
+      </c>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
       <c r="S4" s="19"/>
@@ -1108,6 +1133,18 @@
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="K5" t="s">
+        <v>116</v>
+      </c>
+      <c r="L5" t="s">
+        <v>115</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P5" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -1125,6 +1162,18 @@
       <c r="G6" s="27"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
+      </c>
+      <c r="K6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P6" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
@@ -1815,9 +1864,11 @@
     <hyperlink ref="B14" r:id="rId21" xr:uid="{8FA66079-3753-47E9-B090-2503163763E2}"/>
     <hyperlink ref="M12" r:id="rId22" xr:uid="{0A036A2D-396A-4563-AA5D-8BAE50337625}"/>
     <hyperlink ref="M21" r:id="rId23" xr:uid="{487E3C3E-3BEA-4A39-8CC2-A2E909E780A4}"/>
+    <hyperlink ref="M5" r:id="rId24" xr:uid="{6D2BF177-69AB-4F23-A4E4-952DD670CEDF}"/>
+    <hyperlink ref="M6" r:id="rId25" xr:uid="{F4485923-6E80-4131-9611-17585253A4EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add: 22Ohm USB Data-Line series resistor.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673AED6E-97F9-45D6-93D6-6448749DBC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4E44E5-498C-4A92-A7ED-24B88063A1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="124">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>22Ohm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/vishay-dale/RCS060322R0JNEA/541-2809-1-ND/5867102</t>
   </si>
 </sst>
 </file>
@@ -605,10 +611,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -617,19 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -987,7 +993,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7:R7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,57 +1005,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="L1" s="25" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="L1" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26" t="s">
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1058,16 +1064,16 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>104</v>
@@ -1075,61 +1081,61 @@
       <c r="L3" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="Q3" s="22"/>
-      <c r="R3" s="22"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
       <c r="S3" s="19"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
       <c r="K4" t="s">
         <v>103</v>
       </c>
       <c r="L4" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="22"/>
-      <c r="O4" s="22"/>
-      <c r="P4" s="22" t="s">
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="Q4" s="22"/>
-      <c r="R4" s="22"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
       <c r="S4" s="19"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26" t="s">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1150,16 +1156,16 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1177,39 +1183,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
       <c r="L7" s="19"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="22"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
       <c r="S7" s="19"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1218,72 +1224,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="L10" s="25" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="L10" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="26" t="s">
+      <c r="M11" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26" t="s">
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="26"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1292,108 +1298,117 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="8" t="s">
         <v>17</v>
+      </c>
+      <c r="L13" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="P13" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="L15" s="25" t="s">
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="L15" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="26" t="s">
+      <c r="M16" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26" t="s">
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1402,87 +1417,87 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
       <c r="L17" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="22"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="19"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L18" s="19"/>
-      <c r="M18" s="21"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="22"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
       <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="L19" s="25" t="s">
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="L19" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="M19" s="25"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="25"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26" t="s">
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="26" t="s">
+      <c r="M20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26" t="s">
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
       <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1491,16 +1506,16 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="23" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
@@ -1510,42 +1525,42 @@
       <c r="L21" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="M21" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="22"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
       <c r="S21" s="19"/>
     </row>
     <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1554,76 +1569,76 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26" t="s">
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26" t="s">
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1635,16 +1650,16 @@
       <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="23" t="s">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -1653,154 +1668,129 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="21" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26" t="s">
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="19"/>
-      <c r="B36" s="22"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="22"/>
-      <c r="E36" s="22"/>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
       <c r="H36" s="19"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="25" t="s">
+      <c r="A38" s="21" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26" t="s">
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="19"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="20"/>
-      <c r="B41" s="29"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="29"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="L19:S19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="A7:H7"/>
@@ -1817,28 +1807,53 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{29E80626-A7A5-45E8-8609-3380F35C4604}"/>
@@ -1866,9 +1881,10 @@
     <hyperlink ref="M21" r:id="rId23" xr:uid="{487E3C3E-3BEA-4A39-8CC2-A2E909E780A4}"/>
     <hyperlink ref="M5" r:id="rId24" xr:uid="{6D2BF177-69AB-4F23-A4E4-952DD670CEDF}"/>
     <hyperlink ref="M6" r:id="rId25" xr:uid="{F4485923-6E80-4131-9611-17585253A4EF}"/>
+    <hyperlink ref="M13" r:id="rId26" xr:uid="{C3262577-DD79-4432-9AAB-17157479D48E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add: LEDLadder and Switch Matrix Schematics. LEDLadder schematic completed. Encoder and 150Ohm Resistor components.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4E44E5-498C-4A92-A7ED-24B88063A1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837EE0B0-8FD0-4092-8DE1-3D1630190829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="127">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>https://www.digikey.com.au/product-detail/en/vishay-dale/RCS060322R0JNEA/541-2809-1-ND/5867102</t>
+  </si>
+  <si>
+    <t>150Ohm</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/vishay-dale/CRCW0603150RFKEAHP/541-150SCT-ND/2825983</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -577,7 +586,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -638,6 +647,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -993,7 +1006,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,8 +1356,8 @@
       <c r="M13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="P13" t="s">
-        <v>121</v>
+      <c r="P13" s="31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1356,6 +1369,15 @@
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
+      <c r="L14" t="s">
+        <v>124</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="P14" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A15" s="21" t="s">
@@ -1569,7 +1591,7 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="30" t="s">
         <v>36</v>
       </c>
       <c r="C25" s="26"/>
@@ -1882,9 +1904,10 @@
     <hyperlink ref="M5" r:id="rId24" xr:uid="{6D2BF177-69AB-4F23-A4E4-952DD670CEDF}"/>
     <hyperlink ref="M6" r:id="rId25" xr:uid="{F4485923-6E80-4131-9611-17585253A4EF}"/>
     <hyperlink ref="M13" r:id="rId26" xr:uid="{C3262577-DD79-4432-9AAB-17157479D48E}"/>
+    <hyperlink ref="M14" r:id="rId27" xr:uid="{7B2B2DB7-3570-4A4F-A9A9-B48A2EF011FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add: Encoder component added to schematic and pin-list.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{837EE0B0-8FD0-4092-8DE1-3D1630190829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FEF02B-73D0-471B-B399-598FEC2565CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -408,6 +408,42 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>RGB LED Control</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>Encoder Button</t>
+  </si>
+  <si>
+    <t>Encoder A</t>
+  </si>
+  <si>
+    <t>IN/INT</t>
+  </si>
+  <si>
+    <t>Encoder B</t>
+  </si>
+  <si>
+    <t>PCINT4</t>
+  </si>
+  <si>
+    <t>PCINT5</t>
+  </si>
+  <si>
+    <t>PCINT6</t>
   </si>
 </sst>
 </file>
@@ -606,17 +642,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
@@ -651,6 +684,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -1005,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -1018,57 +1060,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="L1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="L1" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22" t="s">
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1077,78 +1119,78 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>104</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="23" t="s">
+      <c r="M3" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24" t="s">
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="19"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
       <c r="K4" t="s">
         <v>103</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24" t="s">
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="19"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1169,16 +1211,16 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1196,39 +1238,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="24"/>
-      <c r="S7" s="19"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1237,72 +1279,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="L10" s="21" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="L10" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="22" t="s">
+      <c r="M11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22" t="s">
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1311,42 +1353,42 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="28"/>
-      <c r="O12" s="28"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
       <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1356,7 +1398,7 @@
       <c r="M13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="P13" s="31" t="s">
+      <c r="P13" s="28" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1364,11 +1406,11 @@
       <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
       <c r="L14" t="s">
         <v>124</v>
       </c>
@@ -1380,57 +1422,57 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="L15" s="21" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="L15" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="21"/>
-      <c r="S15" s="21"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22" t="s">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22" t="s">
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="22"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1439,87 +1481,87 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="L17" s="19" t="s">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="L17" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="M17" s="23" t="s">
+      <c r="M17" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="19"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="L18" s="19"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="19"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="L19" s="21" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="18"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="L19" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="M19" s="21"/>
-      <c r="N19" s="21"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="21"/>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="21"/>
-      <c r="S19" s="21"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="18"/>
+      <c r="O19" s="18"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="22" t="s">
+      <c r="M20" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22" t="s">
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="22"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
       <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1528,61 +1570,61 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="27" t="s">
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
       <c r="I21" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="19" t="s">
+      <c r="L21" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="M21" s="23" t="s">
+      <c r="M21" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="24"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="19"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="16"/>
     </row>
     <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1591,76 +1633,76 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26" t="s">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22" t="s">
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22" t="s">
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1672,16 +1714,16 @@
       <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="27" t="s">
+      <c r="C32" s="25"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -1690,104 +1732,104 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22" t="s">
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="19"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="20"/>
+      <c r="A37" s="17"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="21" t="s">
+      <c r="A38" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22" t="s">
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="19"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="19"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="20"/>
+      <c r="A41" s="17"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="22"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="85">
@@ -1913,19 +1955,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E8419F-E47E-4ECC-9C6A-0CA831B8893B}">
-  <dimension ref="A2:D35"/>
+  <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>48</v>
       </c>
@@ -1935,415 +1979,507 @@
       <c r="C3" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>1</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
-        <v>1</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="11">
+        <v>2</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>2</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="11">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>3</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11">
+        <v>4</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>4</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>5</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="11">
+        <v>6</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="30"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>7</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="30"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="30"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="11">
+        <v>9</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
+        <v>10</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>11</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="12"/>
+      <c r="F14" s="30"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="30"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
+        <v>13</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="30"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>14</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="30"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>15</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="30"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>16</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="30"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>17</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="30"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>18</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>5</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="E21" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>19</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="F22" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>20</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>21</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>22</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>6</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
+      <c r="E25" s="12"/>
+      <c r="F25" s="30"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>23</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>7</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="14" t="s">
+      <c r="E26" s="12"/>
+      <c r="F26" s="30"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>24</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>8</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="E27" s="12"/>
+      <c r="F27" s="30"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>25</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>9</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14" t="s">
+      <c r="E28" s="12"/>
+      <c r="F28" s="30"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>26</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
-        <v>10</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="14" t="s">
+      <c r="E29" s="12"/>
+      <c r="F29" s="30"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>27</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
-        <v>11</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>12</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>13</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>14</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>15</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
-        <v>16</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
-        <v>17</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>18</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>19</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>20</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>21</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>22</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>23</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
-        <v>24</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12">
-        <v>25</v>
-      </c>
-      <c r="B28" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12">
-        <v>26</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12">
-        <v>27</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="12">
+      <c r="E30" s="12"/>
+      <c r="F30" s="30"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
         <v>28</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="14" t="s">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12">
+      <c r="E31" s="12"/>
+      <c r="F31" s="30"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
         <v>29</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14" t="s">
+      <c r="C32" s="12"/>
+      <c r="D32" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12">
+      <c r="E32" s="12"/>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>30</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="14" t="s">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12">
+      <c r="E33" s="12"/>
+      <c r="F33" s="30"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="11">
         <v>31</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14" t="s">
+      <c r="C34" s="12"/>
+      <c r="D34" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15">
+      <c r="E34" s="12"/>
+      <c r="F34" s="30"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="13">
         <v>32</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17" t="s">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
         <v>83</v>
       </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="31"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D35">

</xml_diff>

<commit_message>
Add: CherryMX Switch and Rectifier Diode Components.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59FEF02B-73D0-471B-B399-598FEC2565CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D8D078-75B3-45EE-8DB7-C099CF20140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="145">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -444,6 +444,24 @@
   </si>
   <si>
     <t>PCINT6</t>
+  </si>
+  <si>
+    <t>Header Pins (16)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/amphenol-icc-fci/67996-416HLF/609-3220-ND/1878538</t>
+  </si>
+  <si>
+    <t>67996-416HLF</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/vishay-general-semiconductor-diodes-division/ES07D-GS08/ES07D-GS08CT-ND/3104461</t>
+  </si>
+  <si>
+    <t>Rectifier Diode</t>
+  </si>
+  <si>
+    <t>ES07D-GS08</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1063,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1500,7 +1518,7 @@
       <c r="R17" s="21"/>
       <c r="S17" s="16"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L18" s="16"/>
       <c r="M18" s="20"/>
       <c r="N18" s="21"/>
@@ -1510,7 +1528,7 @@
       <c r="R18" s="21"/>
       <c r="S18" s="16"/>
     </row>
-    <row r="19" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
@@ -1532,7 +1550,7 @@
       <c r="R19" s="18"/>
       <c r="S19" s="18"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
@@ -1566,7 +1584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1599,7 +1617,7 @@
       <c r="R21" s="21"/>
       <c r="S21" s="16"/>
     </row>
-    <row r="23" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A23" s="18" t="s">
         <v>13</v>
       </c>
@@ -1610,8 +1628,18 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L23" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
@@ -1628,8 +1656,24 @@
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
@@ -1646,8 +1690,20 @@
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="L25" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="M25" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="16"/>
+    </row>
+    <row r="26" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A26" s="18" t="s">
         <v>18</v>
       </c>
@@ -1658,8 +1714,18 @@
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
       <c r="H26" s="18"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L26" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
@@ -1676,8 +1742,41 @@
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" ht="21" x14ac:dyDescent="0.35">
+      <c r="L27" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="L28" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="M28" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="16"/>
+      <c r="X28" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>19</v>
       </c>
@@ -1689,7 +1788,7 @@
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
@@ -1710,7 +1809,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
@@ -1832,7 +1931,17 @@
       <c r="H41" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="85">
+  <mergeCells count="95">
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
     <mergeCell ref="M17:O17"/>
     <mergeCell ref="P17:R17"/>
     <mergeCell ref="M18:O18"/>
@@ -1947,9 +2056,12 @@
     <hyperlink ref="M6" r:id="rId25" xr:uid="{F4485923-6E80-4131-9611-17585253A4EF}"/>
     <hyperlink ref="M13" r:id="rId26" xr:uid="{C3262577-DD79-4432-9AAB-17157479D48E}"/>
     <hyperlink ref="M14" r:id="rId27" xr:uid="{7B2B2DB7-3570-4A4F-A9A9-B48A2EF011FD}"/>
+    <hyperlink ref="M25" r:id="rId28" xr:uid="{60B19C51-3BA4-44DA-B587-F9E53CBF5D75}"/>
+    <hyperlink ref="M28" r:id="rId29" xr:uid="{0220D5E4-1676-43C9-9611-FDBC7B441ABC}"/>
+    <hyperlink ref="X28" r:id="rId30" xr:uid="{DF062097-78AF-434A-8CF8-49E6C08266BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId31"/>
 </worksheet>
 </file>
 
@@ -1957,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E8419F-E47E-4ECC-9C6A-0CA831B8893B}">
   <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Layout of major components complete. TODO: Passive components. TODO: Fix DRC errors in micro-usb footprint.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D8D078-75B3-45EE-8DB7-C099CF20140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0332B5E0-5311-47D1-8FF6-511077D8C23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -671,6 +671,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -683,16 +693,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
@@ -701,15 +708,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R37" sqref="R37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,57 +1078,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="L1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="L1" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1137,16 +1137,16 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>104</v>
@@ -1154,61 +1154,61 @@
       <c r="L3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21" t="s">
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
       <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="K4" t="s">
         <v>103</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21" t="s">
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="21"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1229,16 +1229,16 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1256,39 +1256,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21"/>
-      <c r="P7" s="21"/>
-      <c r="Q7" s="21"/>
-      <c r="R7" s="21"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1297,72 +1297,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23" t="s">
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="L10" s="18" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="L10" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="19"/>
-      <c r="O11" s="19"/>
-      <c r="P11" s="19" t="s">
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="19"/>
-      <c r="R11" s="19"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1371,42 +1371,42 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23" t="s">
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>110</v>
       </c>
-      <c r="M12" s="24" t="s">
+      <c r="M12" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="M13" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="P13" s="28" t="s">
+      <c r="P13" s="18" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1424,11 +1424,11 @@
       <c r="A14" t="s">
         <v>109</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
       <c r="L14" t="s">
         <v>124</v>
       </c>
@@ -1440,57 +1440,57 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="L15" s="18" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="L15" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="19" t="s">
+      <c r="M16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="19"/>
-      <c r="O16" s="19"/>
-      <c r="P16" s="19" t="s">
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="19"/>
-      <c r="R16" s="19"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1499,87 +1499,87 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
       <c r="L17" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="M17" s="20" t="s">
+      <c r="M17" s="24" t="s">
         <v>106</v>
       </c>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="21"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L18" s="16"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="21"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="21"/>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="21"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="L19" s="18" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="L19" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="M19" s="18"/>
-      <c r="N19" s="18"/>
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19" t="s">
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="19" t="s">
+      <c r="M20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19" t="s">
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
       <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1588,16 +1588,16 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="24" t="s">
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
@@ -1607,68 +1607,68 @@
       <c r="L21" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="M21" s="20" t="s">
+      <c r="M21" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
       <c r="S21" s="16"/>
     </row>
     <row r="23" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="L23" s="18" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="L23" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M24" s="19" t="s">
+      <c r="M24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="19"/>
-      <c r="O24" s="19"/>
-      <c r="P24" s="19" t="s">
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="19"/>
-      <c r="R24" s="19"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
       <c r="S24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1677,84 +1677,84 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23" t="s">
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="N25" s="21"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="21"/>
-      <c r="Q25" s="21"/>
-      <c r="R25" s="21"/>
+      <c r="N25" s="25"/>
+      <c r="O25" s="25"/>
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
       <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="L26" s="18" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="L26" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
-      <c r="S26" s="18"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19" t="s">
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="19" t="s">
+      <c r="M27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19" t="s">
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
       <c r="S27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1763,207 +1763,265 @@
       <c r="L28" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="N28" s="21"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="21"/>
-      <c r="Q28" s="21"/>
-      <c r="R28" s="21"/>
+      <c r="N28" s="25"/>
+      <c r="O28" s="25"/>
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
       <c r="S28" s="16"/>
       <c r="X28" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="L30" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19" t="s">
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I31" t="s">
         <v>46</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M31" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
+      <c r="S31" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="25"/>
-      <c r="D32" s="25"/>
-      <c r="E32" s="24" t="s">
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="L32" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="M32" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="16"/>
     </row>
     <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="18"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="16"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
       <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="18"/>
-      <c r="H38" s="18"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="19" t="s">
+      <c r="B39" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19" t="s">
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
       <c r="H41" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="95">
-    <mergeCell ref="L26:S26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="L23:S23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
+  <mergeCells count="100">
+    <mergeCell ref="L30:S30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="A7:H7"/>
@@ -1980,53 +2038,38 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="L19:S19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{29E80626-A7A5-45E8-8609-3380F35C4604}"/>
@@ -2059,9 +2102,10 @@
     <hyperlink ref="M25" r:id="rId28" xr:uid="{60B19C51-3BA4-44DA-B587-F9E53CBF5D75}"/>
     <hyperlink ref="M28" r:id="rId29" xr:uid="{0220D5E4-1676-43C9-9611-FDBC7B441ABC}"/>
     <hyperlink ref="X28" r:id="rId30" xr:uid="{DF062097-78AF-434A-8CF8-49E6C08266BD}"/>
+    <hyperlink ref="M32" r:id="rId31" xr:uid="{F66FADFC-636D-4F41-9E40-03F0BE8F2D98}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -2097,7 +2141,7 @@
       <c r="E3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="19" t="s">
         <v>130</v>
       </c>
     </row>
@@ -2113,7 +2157,7 @@
         <v>83</v>
       </c>
       <c r="E4" s="12"/>
-      <c r="F4" s="30"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
@@ -2127,7 +2171,7 @@
         <v>83</v>
       </c>
       <c r="E5" s="12"/>
-      <c r="F5" s="30"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
@@ -2141,7 +2185,7 @@
         <v>83</v>
       </c>
       <c r="E6" s="12"/>
-      <c r="F6" s="30"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
@@ -2155,7 +2199,7 @@
         <v>83</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7" s="30"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
@@ -2171,7 +2215,7 @@
         <v>84</v>
       </c>
       <c r="E8" s="12"/>
-      <c r="F8" s="30"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
@@ -2185,7 +2229,7 @@
         <v>84</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="30"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
@@ -2201,7 +2245,7 @@
         <v>84</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="30"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
@@ -2217,7 +2261,7 @@
         <v>84</v>
       </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="30"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
@@ -2231,7 +2275,7 @@
         <v>84</v>
       </c>
       <c r="E12" s="12"/>
-      <c r="F12" s="30"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
@@ -2247,7 +2291,7 @@
         <v>84</v>
       </c>
       <c r="E13" s="12"/>
-      <c r="F13" s="30"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
@@ -2263,7 +2307,7 @@
         <v>84</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="F14" s="30"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
@@ -2279,7 +2323,7 @@
         <v>84</v>
       </c>
       <c r="E15" s="12"/>
-      <c r="F15" s="30"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
@@ -2295,7 +2339,7 @@
         <v>84</v>
       </c>
       <c r="E16" s="12"/>
-      <c r="F16" s="30"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
@@ -2311,7 +2355,7 @@
         <v>84</v>
       </c>
       <c r="E17" s="12"/>
-      <c r="F17" s="30"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
@@ -2327,7 +2371,7 @@
         <v>84</v>
       </c>
       <c r="E18" s="12"/>
-      <c r="F18" s="30"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
@@ -2343,7 +2387,7 @@
         <v>84</v>
       </c>
       <c r="E19" s="12"/>
-      <c r="F19" s="30"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
@@ -2359,7 +2403,7 @@
         <v>84</v>
       </c>
       <c r="E20" s="12"/>
-      <c r="F20" s="30"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
@@ -2377,7 +2421,7 @@
       <c r="E21" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2397,7 +2441,7 @@
       <c r="E22" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2417,7 +2461,7 @@
       <c r="E23" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="20" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2435,7 +2479,7 @@
       <c r="E24" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="20" t="s">
         <v>131</v>
       </c>
     </row>
@@ -2451,7 +2495,7 @@
         <v>84</v>
       </c>
       <c r="E25" s="12"/>
-      <c r="F25" s="30"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
@@ -2465,7 +2509,7 @@
         <v>84</v>
       </c>
       <c r="E26" s="12"/>
-      <c r="F26" s="30"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
@@ -2479,7 +2523,7 @@
         <v>84</v>
       </c>
       <c r="E27" s="12"/>
-      <c r="F27" s="30"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
@@ -2493,7 +2537,7 @@
         <v>84</v>
       </c>
       <c r="E28" s="12"/>
-      <c r="F28" s="30"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
@@ -2507,7 +2551,7 @@
         <v>84</v>
       </c>
       <c r="E29" s="12"/>
-      <c r="F29" s="30"/>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
@@ -2521,7 +2565,7 @@
         <v>84</v>
       </c>
       <c r="E30" s="12"/>
-      <c r="F30" s="30"/>
+      <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
@@ -2535,7 +2579,7 @@
         <v>83</v>
       </c>
       <c r="E31" s="12"/>
-      <c r="F31" s="30"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
@@ -2549,7 +2593,7 @@
         <v>83</v>
       </c>
       <c r="E32" s="12"/>
-      <c r="F32" s="30"/>
+      <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
@@ -2563,7 +2607,7 @@
         <v>83</v>
       </c>
       <c r="E33" s="12"/>
-      <c r="F33" s="30"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
@@ -2577,7 +2621,7 @@
         <v>83</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="F34" s="30"/>
+      <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="13">
@@ -2591,7 +2635,7 @@
         <v>83</v>
       </c>
       <c r="E35" s="14"/>
-      <c r="F35" s="31"/>
+      <c r="F35" s="21"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:D35">

</xml_diff>

<commit_message>
Add: altium-library component library. Add: Standoffs in component list. NOT IN PCB YET. Progress: PCB Layout in progress.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0332B5E0-5311-47D1-8FF6-511077D8C23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB56DE9-4F2F-43A3-B896-3D9112A49DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="147">
   <si>
     <t>Microprocessor Selection</t>
   </si>
@@ -158,12 +158,6 @@
     <t>I have some of these already</t>
   </si>
   <si>
-    <t>USB3076-30-A</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com.au/product-detail/en/gct/USB3076-30-A/2073-USB3076-30-ACT-ND/9859706</t>
-  </si>
-  <si>
     <t>https://gct.co/files/specs/usb3076-spec.pdf</t>
   </si>
   <si>
@@ -462,6 +456,18 @@
   </si>
   <si>
     <t>ES07D-GS08</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/raf-electronic-hardware/M2101-3005-AL/1772-1936-ND/7681347</t>
+  </si>
+  <si>
+    <t>Standoffs</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com.au/product-detail/en/10118193-0001LF/609-4616-1-ND/2785380?utm_campaign=buynow&amp;utm_medium=aggregator&amp;curr=usd&amp;utm_source=octopart</t>
+  </si>
+  <si>
+    <t>10118193-0001LF</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -693,23 +699,29 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1065,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,7 +1101,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
       <c r="L1" s="22" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
@@ -1137,30 +1149,30 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M3" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
       <c r="P3" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q3" s="25"/>
       <c r="R3" s="25"/>
@@ -1178,18 +1190,18 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
       <c r="K4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L4" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M4" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N4" s="25"/>
       <c r="O4" s="25"/>
       <c r="P4" s="25" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Q4" s="25"/>
       <c r="R4" s="25"/>
@@ -1213,46 +1225,46 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L5" t="s">
+        <v>113</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="M5" s="4" t="s">
-        <v>117</v>
-      </c>
       <c r="P5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28" t="s">
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
       <c r="K6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="M6" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="P6" t="s">
         <v>119</v>
-      </c>
-      <c r="P6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
@@ -1297,16 +1309,16 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28" t="s">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
@@ -1323,7 +1335,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="L10" s="22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
@@ -1371,72 +1383,72 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28" t="s">
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
-        <v>110</v>
-      </c>
-      <c r="M12" s="26" t="s">
-        <v>111</v>
-      </c>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
+        <v>108</v>
+      </c>
+      <c r="M12" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="N12" s="30"/>
+      <c r="O12" s="30"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
       <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
       <c r="L13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P13" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
+        <v>107</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
       <c r="L14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="P14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
@@ -1451,7 +1463,7 @@
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="L15" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -1499,17 +1511,17 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
       <c r="L17" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M17" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N17" s="25"/>
       <c r="O17" s="25"/>
@@ -1540,7 +1552,7 @@
       <c r="G19" s="22"/>
       <c r="H19" s="22"/>
       <c r="L19" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
@@ -1588,16 +1600,16 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="26" t="s">
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="30"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
@@ -1605,10 +1617,10 @@
         <v>41</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="M21" s="24" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="N21" s="25"/>
       <c r="O21" s="25"/>
@@ -1629,7 +1641,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="L23" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
@@ -1677,24 +1689,24 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28" t="s">
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="M25" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N25" s="25"/>
       <c r="O25" s="25"/>
@@ -1715,7 +1727,7 @@
       <c r="G26" s="22"/>
       <c r="H26" s="22"/>
       <c r="L26" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M26" s="22"/>
       <c r="N26" s="22"/>
@@ -1761,10 +1773,10 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L28" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M28" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N28" s="25"/>
       <c r="O28" s="25"/>
@@ -1773,7 +1785,7 @@
       <c r="R28" s="25"/>
       <c r="S28" s="16"/>
       <c r="X28" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.35">
@@ -1788,7 +1800,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
       <c r="L30" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M30" s="22"/>
       <c r="N30" s="22"/>
@@ -1816,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="I31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L31" s="2" t="s">
         <v>1</v>
@@ -1837,29 +1849,29 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>146</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="27"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" s="27"/>
-      <c r="G32" s="27"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M32" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="N32" s="25"/>
       <c r="O32" s="25"/>
@@ -1868,9 +1880,9 @@
       <c r="R32" s="25"/>
       <c r="S32" s="16"/>
     </row>
-    <row r="34" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A34" s="22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B34" s="22"/>
       <c r="C34" s="22"/>
@@ -1879,8 +1891,18 @@
       <c r="F34" s="22"/>
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L34" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
@@ -1897,8 +1919,24 @@
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="L35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
       <c r="B36" s="25"/>
       <c r="C36" s="25"/>
@@ -1907,20 +1945,25 @@
       <c r="F36" s="25"/>
       <c r="G36" s="25"/>
       <c r="H36" s="16"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="M36" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="N36" s="32"/>
+      <c r="O36" s="32"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
       <c r="H37" s="17"/>
     </row>
-    <row r="38" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:19" ht="21" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -1930,7 +1973,7 @@
       <c r="G38" s="22"/>
       <c r="H38" s="22"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
@@ -1948,7 +1991,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -1958,70 +2001,54 @@
       <c r="G40" s="25"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
       <c r="H41" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
-    <mergeCell ref="L30:S30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="L19:S19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
+  <mergeCells count="104">
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="L34:S34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="L1:S1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="P3:R3"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="A7:H7"/>
@@ -2038,38 +2065,58 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="L1:S1"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M3:O3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="L23:S23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="L26:S26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="L30:S30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{29E80626-A7A5-45E8-8609-3380F35C4604}"/>
@@ -2103,9 +2150,10 @@
     <hyperlink ref="M28" r:id="rId29" xr:uid="{0220D5E4-1676-43C9-9611-FDBC7B441ABC}"/>
     <hyperlink ref="X28" r:id="rId30" xr:uid="{DF062097-78AF-434A-8CF8-49E6C08266BD}"/>
     <hyperlink ref="M32" r:id="rId31" xr:uid="{F66FADFC-636D-4F41-9E40-03F0BE8F2D98}"/>
+    <hyperlink ref="M36" r:id="rId32" xr:uid="{5A62746B-C831-49DF-9323-787E643971F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId32"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId33"/>
 </worksheet>
 </file>
 
@@ -2127,22 +2175,22 @@
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2150,11 +2198,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="20"/>
@@ -2164,11 +2212,11 @@
         <v>2</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="20"/>
@@ -2178,11 +2226,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="20"/>
@@ -2192,11 +2240,11 @@
         <v>4</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="20"/>
@@ -2206,13 +2254,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="20"/>
@@ -2222,11 +2270,11 @@
         <v>6</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="20"/>
@@ -2236,13 +2284,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="20"/>
@@ -2252,13 +2300,13 @@
         <v>8</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="20"/>
@@ -2268,11 +2316,11 @@
         <v>9</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="20"/>
@@ -2282,13 +2330,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="20"/>
@@ -2298,13 +2346,13 @@
         <v>11</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="20"/>
@@ -2314,13 +2362,13 @@
         <v>12</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="20"/>
@@ -2330,13 +2378,13 @@
         <v>13</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E16" s="12"/>
       <c r="F16" s="20"/>
@@ -2346,13 +2394,13 @@
         <v>14</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="20"/>
@@ -2362,13 +2410,13 @@
         <v>15</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="20"/>
@@ -2378,13 +2426,13 @@
         <v>16</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="20"/>
@@ -2394,13 +2442,13 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="20"/>
@@ -2410,19 +2458,19 @@
         <v>18</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F21" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2430,19 +2478,19 @@
         <v>19</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F22" s="20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2450,19 +2498,19 @@
         <v>20</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F23" s="20" t="s">
         <v>132</v>
-      </c>
-      <c r="F23" s="20" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -2470,17 +2518,17 @@
         <v>21</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E24" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="20" t="s">
         <v>129</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2488,11 +2536,11 @@
         <v>22</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="20"/>
@@ -2502,11 +2550,11 @@
         <v>23</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="20"/>
@@ -2516,11 +2564,11 @@
         <v>24</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="20"/>
@@ -2530,11 +2578,11 @@
         <v>25</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="20"/>
@@ -2544,11 +2592,11 @@
         <v>26</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="20"/>
@@ -2558,11 +2606,11 @@
         <v>27</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C30" s="12"/>
       <c r="D30" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="20"/>
@@ -2572,11 +2620,11 @@
         <v>28</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C31" s="12"/>
       <c r="D31" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="20"/>
@@ -2586,11 +2634,11 @@
         <v>29</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C32" s="12"/>
       <c r="D32" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="20"/>
@@ -2600,11 +2648,11 @@
         <v>30</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="20"/>
@@ -2614,11 +2662,11 @@
         <v>31</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="20"/>
@@ -2628,11 +2676,11 @@
         <v>32</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C35" s="14"/>
       <c r="D35" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E35" s="14"/>
       <c r="F35" s="21"/>

</xml_diff>

<commit_message>
Update: Board Layout V1 complete. TODO: VCC and GND connections to polygon fill.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB56DE9-4F2F-43A3-B896-3D9112A49DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28F7C46-54E6-4066-BDCA-BC8EDA59AF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Components" sheetId="1" r:id="rId1"/>
@@ -687,6 +687,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -699,29 +705,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1077,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:D32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,57 +1090,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="L1" s="22" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="L1" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23" t="s">
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="23"/>
-      <c r="R2" s="23"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1149,16 +1149,16 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27" t="s">
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>102</v>
@@ -1166,61 +1166,61 @@
       <c r="L3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25" t="s">
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
       <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
       <c r="K4" t="s">
         <v>101</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="24" t="s">
+      <c r="M4" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25" t="s">
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1241,16 +1241,16 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1268,39 +1268,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="O7" s="25"/>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="27"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1309,72 +1309,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="L10" s="22" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="L10" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23" t="s">
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1383,27 +1383,27 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27" t="s">
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>108</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N12" s="30"/>
-      <c r="O12" s="30"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -1436,11 +1436,11 @@
       <c r="A14" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
       <c r="L14" t="s">
         <v>122</v>
       </c>
@@ -1452,57 +1452,57 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="L15" s="22" t="s">
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="24"/>
+      <c r="L15" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="22"/>
-      <c r="S15" s="22"/>
+      <c r="M15" s="24"/>
+      <c r="N15" s="24"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23" t="s">
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23" t="s">
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1511,87 +1511,87 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
       <c r="L17" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L18" s="16"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="25"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
+      <c r="R18" s="27"/>
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="L19" s="22" t="s">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="L19" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23" t="s">
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23" t="s">
+      <c r="N20" s="25"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
       <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1600,16 +1600,16 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="29" t="s">
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
@@ -1619,68 +1619,68 @@
       <c r="L21" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="M21" s="24" t="s">
+      <c r="M21" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="27"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
       <c r="S21" s="16"/>
     </row>
     <row r="23" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="L23" s="22" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="L23" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="22"/>
-      <c r="S23" s="22"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="24"/>
+      <c r="Q23" s="24"/>
+      <c r="R23" s="24"/>
+      <c r="S23" s="24"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23" t="s">
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23" t="s">
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
       <c r="S24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1689,84 +1689,84 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27" t="s">
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="M25" s="24" t="s">
+      <c r="M25" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="25"/>
+      <c r="N25" s="27"/>
+      <c r="O25" s="27"/>
+      <c r="P25" s="27"/>
+      <c r="Q25" s="27"/>
+      <c r="R25" s="27"/>
       <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
-      <c r="L26" s="22" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="L26" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
+      <c r="S26" s="24"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23" t="s">
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="23" t="s">
+      <c r="M27" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23" t="s">
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
       <c r="S27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1775,55 +1775,55 @@
       <c r="L28" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M28" s="24" t="s">
+      <c r="M28" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="N28" s="25"/>
-      <c r="O28" s="25"/>
-      <c r="P28" s="25"/>
-      <c r="Q28" s="25"/>
-      <c r="R28" s="25"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="27"/>
+      <c r="Q28" s="27"/>
+      <c r="R28" s="27"/>
       <c r="S28" s="16"/>
       <c r="X28" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
-      <c r="L30" s="22" t="s">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="L30" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
-      <c r="O30" s="22"/>
-      <c r="P30" s="22"/>
-      <c r="Q30" s="22"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
+      <c r="M30" s="24"/>
+      <c r="N30" s="24"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="24"/>
+      <c r="R30" s="24"/>
+      <c r="S30" s="24"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23" t="s">
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+      <c r="E31" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1833,16 +1833,16 @@
       <c r="L31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M31" s="23" t="s">
+      <c r="M31" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23" t="s">
+      <c r="N31" s="25"/>
+      <c r="O31" s="25"/>
+      <c r="P31" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
       <c r="S31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1851,16 +1851,16 @@
       <c r="A32" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="29" t="s">
+      <c r="B32" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="30"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="29" t="s">
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -1870,180 +1870,182 @@
       <c r="L32" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M32" s="24" t="s">
+      <c r="M32" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="N32" s="25"/>
-      <c r="O32" s="25"/>
-      <c r="P32" s="25"/>
-      <c r="Q32" s="25"/>
-      <c r="R32" s="25"/>
+      <c r="N32" s="27"/>
+      <c r="O32" s="27"/>
+      <c r="P32" s="27"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="27"/>
       <c r="S32" s="16"/>
     </row>
     <row r="34" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="22"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="22"/>
-      <c r="L34" s="22" t="s">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="L34" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
-      <c r="Q34" s="22"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
+      <c r="M34" s="24"/>
+      <c r="N34" s="24"/>
+      <c r="O34" s="24"/>
+      <c r="P34" s="24"/>
+      <c r="Q34" s="24"/>
+      <c r="R34" s="24"/>
+      <c r="S34" s="24"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23" t="s">
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M35" s="23" t="s">
+      <c r="M35" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="N35" s="23"/>
-      <c r="O35" s="23"/>
-      <c r="P35" s="23" t="s">
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="Q35" s="23"/>
-      <c r="R35" s="23"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
       <c r="S35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
       <c r="H36" s="16"/>
-      <c r="M36" s="33" t="s">
+      <c r="M36" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="N36" s="32"/>
-      <c r="O36" s="32"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="33"/>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
       <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23" t="s">
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="26"/>
-      <c r="G41" s="26"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="33"/>
+      <c r="E41" s="33"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="33"/>
       <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="L34:S34"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="L26:S26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="L23:S23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="L1:S1"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:R2"/>
@@ -2068,50 +2070,48 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
     <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="A10:H10"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="E12:G12"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
     <mergeCell ref="L19:S19"/>
     <mergeCell ref="M20:O20"/>
     <mergeCell ref="P20:R20"/>
     <mergeCell ref="M21:O21"/>
     <mergeCell ref="P21:R21"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="L34:S34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
     <mergeCell ref="L30:S30"/>
     <mergeCell ref="M31:O31"/>
     <mergeCell ref="P31:R31"/>

</xml_diff>

<commit_message>
Add: Manufacturing outputs generated.
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Electronics\media-controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28F7C46-54E6-4066-BDCA-BC8EDA59AF21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841F7BAA-CA9A-49E0-920F-B18EDBE9DFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -687,22 +687,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -711,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyAlignment="1">
@@ -720,8 +717,11 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1078,7 +1078,7 @@
   <dimension ref="A1:X41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+      <selection activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,57 +1090,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="L1" s="24" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="L1" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25" t="s">
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
       <c r="S2" s="2" t="s">
         <v>7</v>
       </c>
@@ -1149,16 +1149,16 @@
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
       <c r="H3" s="6"/>
       <c r="K3" t="s">
         <v>102</v>
@@ -1166,61 +1166,61 @@
       <c r="L3" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="26" t="s">
+      <c r="M3" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27" t="s">
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
       <c r="S3" s="16"/>
     </row>
     <row r="4" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
       <c r="K4" t="s">
         <v>101</v>
       </c>
       <c r="L4" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="M4" s="26" t="s">
+      <c r="M4" s="29" t="s">
         <v>100</v>
       </c>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27" t="s">
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
       <c r="S4" s="16"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="H5" s="2" t="s">
         <v>7</v>
       </c>
@@ -1241,16 +1241,16 @@
       <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
       <c r="H6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1268,39 +1268,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="L7" s="16"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
       <c r="S7" s="16"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
       <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1309,72 +1309,72 @@
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30" t="s">
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
       <c r="H9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="L10" s="24" t="s">
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="L10" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="R10" s="24"/>
-      <c r="S10" s="24"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25" t="s">
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
       <c r="H11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M11" s="25" t="s">
+      <c r="M11" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25" t="s">
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
+      <c r="Q11" s="23"/>
+      <c r="R11" s="23"/>
       <c r="S11" s="2" t="s">
         <v>7</v>
       </c>
@@ -1383,42 +1383,42 @@
       <c r="A12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L12" t="s">
         <v>108</v>
       </c>
-      <c r="M12" s="28" t="s">
+      <c r="M12" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="28"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31" t="s">
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="8" t="s">
         <v>17</v>
       </c>
@@ -1436,11 +1436,11 @@
       <c r="A14" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
       <c r="L14" t="s">
         <v>122</v>
       </c>
@@ -1452,57 +1452,57 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="L15" s="24" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="L15" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="22"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25" t="s">
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M16" s="25" t="s">
+      <c r="M16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25" t="s">
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q16" s="25"/>
-      <c r="R16" s="25"/>
+      <c r="Q16" s="23"/>
+      <c r="R16" s="23"/>
       <c r="S16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1511,87 +1511,87 @@
       <c r="A17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
       <c r="L17" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="M17" s="26" t="s">
+      <c r="M17" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="N17" s="27"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="27"/>
-      <c r="Q17" s="27"/>
-      <c r="R17" s="27"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="16"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="L18" s="16"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
       <c r="S18" s="16"/>
     </row>
     <row r="19" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="L19" s="24" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="L19" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="22"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="22"/>
+      <c r="S19" s="22"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25" t="s">
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M20" s="25" t="s">
+      <c r="M20" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N20" s="25"/>
-      <c r="O20" s="25"/>
-      <c r="P20" s="25" t="s">
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="25"/>
-      <c r="R20" s="25"/>
+      <c r="Q20" s="23"/>
+      <c r="R20" s="23"/>
       <c r="S20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1600,16 +1600,16 @@
       <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="28" t="s">
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
       <c r="H21" t="s">
         <v>9</v>
       </c>
@@ -1619,68 +1619,68 @@
       <c r="L21" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="M21" s="26" t="s">
+      <c r="M21" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
       <c r="S21" s="16"/>
     </row>
     <row r="23" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="L23" s="24" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="L23" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-      <c r="O23" s="24"/>
-      <c r="P23" s="24"/>
-      <c r="Q23" s="24"/>
-      <c r="R23" s="24"/>
-      <c r="S23" s="24"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25" t="s">
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M24" s="25" t="s">
+      <c r="M24" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N24" s="25"/>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25" t="s">
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="25"/>
+      <c r="Q24" s="23"/>
+      <c r="R24" s="23"/>
       <c r="S24" s="2" t="s">
         <v>7</v>
       </c>
@@ -1689,84 +1689,84 @@
       <c r="A25" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="30"/>
-      <c r="G25" s="30"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
       <c r="H25" s="6" t="s">
         <v>17</v>
       </c>
       <c r="L25" s="16" t="s">
         <v>139</v>
       </c>
-      <c r="M25" s="26" t="s">
+      <c r="M25" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
       <c r="S25" s="16"/>
     </row>
     <row r="26" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="L26" s="24" t="s">
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="L26" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="24"/>
-      <c r="S26" s="24"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25" t="s">
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M27" s="25" t="s">
+      <c r="M27" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N27" s="25"/>
-      <c r="O27" s="25"/>
-      <c r="P27" s="25" t="s">
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q27" s="25"/>
-      <c r="R27" s="25"/>
+      <c r="Q27" s="23"/>
+      <c r="R27" s="23"/>
       <c r="S27" s="2" t="s">
         <v>7</v>
       </c>
@@ -1775,55 +1775,55 @@
       <c r="L28" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M28" s="26" t="s">
+      <c r="M28" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
+      <c r="N28" s="24"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="24"/>
+      <c r="R28" s="24"/>
       <c r="S28" s="16"/>
       <c r="X28" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A30" s="24" t="s">
+      <c r="A30" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="L30" s="24" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="L30" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="24"/>
-      <c r="S30" s="24"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25" t="s">
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1833,16 +1833,16 @@
       <c r="L31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M31" s="25" t="s">
+      <c r="M31" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25" t="s">
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="25"/>
+      <c r="Q31" s="23"/>
+      <c r="R31" s="23"/>
       <c r="S31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1851,16 +1851,16 @@
       <c r="A32" t="s">
         <v>146</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="28" t="s">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
       <c r="H32" t="s">
         <v>17</v>
       </c>
@@ -1870,182 +1870,196 @@
       <c r="L32" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="M32" s="26" t="s">
+      <c r="M32" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="N32" s="27"/>
-      <c r="O32" s="27"/>
-      <c r="P32" s="27"/>
-      <c r="Q32" s="27"/>
-      <c r="R32" s="27"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
       <c r="S32" s="16"/>
     </row>
     <row r="34" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A34" s="24" t="s">
+      <c r="A34" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="L34" s="24" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="L34" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="M34" s="24"/>
-      <c r="N34" s="24"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22"/>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25" t="s">
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M35" s="25" t="s">
+      <c r="M35" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="N35" s="25"/>
-      <c r="O35" s="25"/>
-      <c r="P35" s="25" t="s">
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="Q35" s="25"/>
-      <c r="R35" s="25"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
       <c r="S35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="16"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="24"/>
       <c r="H36" s="16"/>
-      <c r="M36" s="22" t="s">
+      <c r="M36" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="17"/>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:19" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25" t="s">
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="16"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
       <c r="H40" s="16"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="17"/>
-      <c r="B41" s="33"/>
-      <c r="C41" s="33"/>
-      <c r="D41" s="33"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="33"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="L34:S34"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="L26:S26"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="L30:S30"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="P24:R24"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="P17:R17"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="P18:R18"/>
+    <mergeCell ref="L19:S19"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="P21:R21"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="L15:S15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="L10:S10"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="E16:G16"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="A10:H10"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:G12"/>
     <mergeCell ref="L1:S1"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="P2:R2"/>
@@ -2070,53 +2084,39 @@
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="E25:G25"/>
     <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="L15:S15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="L10:S10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="M7:O7"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="E16:G16"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="A10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:G12"/>
-    <mergeCell ref="L23:S23"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="P24:R24"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="P25:R25"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="P17:R17"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="P18:R18"/>
-    <mergeCell ref="L19:S19"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="L34:S34"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="L26:S26"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="L30:S30"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="E39:G39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{29E80626-A7A5-45E8-8609-3380F35C4604}"/>

</xml_diff>